<commit_message>
Minor change on `AC8B` example file.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_ac8b.xlsx
+++ b/andes/cases/ieee14/ieee14_ac8b.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0144F3-BA9B-9C4A-AEDB-422989CEADF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E35BD4-110D-9B4E-B1EB-D50EA8BC4222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="27320" windowHeight="19980" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="185">
   <si>
     <t>idx</t>
   </si>
@@ -585,6 +585,9 @@
   </si>
   <si>
     <t>VEMIN</t>
+  </si>
+  <si>
+    <t>AC8B_1</t>
   </si>
 </sst>
 </file>
@@ -1930,9 +1933,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="237" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="237" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2026,6 +2029,9 @@
       </c>
       <c r="C2">
         <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>184</v>
       </c>
       <c r="E2" t="s">
         <v>121</v>

</xml_diff>

<commit_message>
Revised `AC8B` example file parameters.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_ac8b.xlsx
+++ b/andes/cases/ieee14/ieee14_ac8b.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E35BD4-110D-9B4E-B1EB-D50EA8BC4222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87F446D-99A4-A04E-914C-86A1D1B6DA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1933,9 +1933,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="237" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2036,6 +2036,15 @@
       <c r="E2" t="s">
         <v>121</v>
       </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
       <c r="T2">
         <v>0</v>
       </c>
@@ -2047,6 +2056,15 @@
       </c>
       <c r="W2">
         <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>